<commit_message>
Make hardmode_percent actually a percentage instead of fraction
</commit_message>
<xml_diff>
--- a/hardmode-stats.xlsx
+++ b/hardmode-stats.xlsx
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.01689197569142999</v>
+        <v>1.689197569142999</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.01736894476025339</v>
+        <v>1.736894476025339</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.0209123604840561</v>
+        <v>2.09123604840561</v>
       </c>
       <c r="F4" t="n">
         <v>1</v>
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.02092706330389979</v>
+        <v>2.092706330389979</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -583,7 +583,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.01960618663893943</v>
+        <v>1.960618663893943</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -607,7 +607,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.02520229646037702</v>
+        <v>2.520229646037702</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -631,7 +631,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.02351254395695169</v>
+        <v>2.351254395695169</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -655,7 +655,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.02261025840295318</v>
+        <v>2.261025840295317</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.02363925213134932</v>
+        <v>2.363925213134932</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -703,7 +703,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.02538288095698862</v>
+        <v>2.538288095698862</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -727,7 +727,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.0280878026702874</v>
+        <v>2.80878026702874</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.02527955755429011</v>
+        <v>2.527955755429011</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -775,7 +775,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.02700808315981046</v>
+        <v>2.700808315981046</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.02706711431462735</v>
+        <v>2.706711431462735</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -823,7 +823,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.02836568125256223</v>
+        <v>2.836568125256223</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.02826669235243342</v>
+        <v>2.826669235243342</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.0322316868058193</v>
+        <v>3.22316868058193</v>
       </c>
       <c r="F18" t="n">
         <v>1</v>
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.03150460919523596</v>
+        <v>3.150460919523596</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -919,7 +919,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.03361358434651461</v>
+        <v>3.361358434651461</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -943,7 +943,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.03450717807162402</v>
+        <v>3.450717807162402</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -967,7 +967,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.03753939818431615</v>
+        <v>3.753939818431615</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.03700913096226294</v>
+        <v>3.700913096226294</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.03910589880110083</v>
+        <v>3.910589880110083</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1039,7 +1039,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.03910475398020591</v>
+        <v>3.910475398020591</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1063,7 +1063,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.03869045080090883</v>
+        <v>3.869045080090883</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1087,7 +1087,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.03925030670778209</v>
+        <v>3.925030670778209</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1111,7 +1111,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.04078721075672295</v>
+        <v>4.078721075672295</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1135,7 +1135,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0.04118394457279963</v>
+        <v>4.118394457279964</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0.04287796608048846</v>
+        <v>4.287796608048846</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.04410034145933676</v>
+        <v>4.410034145933675</v>
       </c>
       <c r="F31" t="n">
         <v>1</v>
@@ -1207,7 +1207,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.04628280389136378</v>
+        <v>4.628280389136378</v>
       </c>
       <c r="F32" t="n">
         <v>1</v>
@@ -1231,7 +1231,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.04570896632127434</v>
+        <v>4.570896632127434</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1255,7 +1255,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0.04534141964554707</v>
+        <v>4.534141964554707</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1279,7 +1279,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0.04422136928779976</v>
+        <v>4.422136928779976</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1303,7 +1303,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.03812772123116209</v>
+        <v>3.812772123116209</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1327,7 +1327,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.0344961742964596</v>
+        <v>3.449617429645961</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1351,7 +1351,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.01170933178602448</v>
+        <v>1.170933178602449</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1375,7 +1375,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.03954940521028904</v>
+        <v>3.954940521028904</v>
       </c>
       <c r="F39" t="n">
         <v>1</v>
@@ -1399,7 +1399,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0.03593365666560124</v>
+        <v>3.593365666560124</v>
       </c>
       <c r="F40" t="n">
         <v>1</v>
@@ -1423,7 +1423,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0.03707014679640067</v>
+        <v>3.707014679640067</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1447,7 +1447,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.03733008189986638</v>
+        <v>3.733008189986638</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1471,7 +1471,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.03853143214773147</v>
+        <v>3.853143214773147</v>
       </c>
       <c r="F43" t="n">
         <v>1</v>
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.03981553305209916</v>
+        <v>3.981553305209916</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
@@ -1519,7 +1519,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.04059186406445522</v>
+        <v>4.059186406445522</v>
       </c>
       <c r="F45" t="n">
         <v>1</v>
@@ -1543,7 +1543,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.03905916457085864</v>
+        <v>3.905916457085864</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.03856297901787463</v>
+        <v>3.856297901787463</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -1591,7 +1591,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.0411094619131337</v>
+        <v>4.11094619131337</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -1615,7 +1615,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.04150809417809585</v>
+        <v>4.150809417809585</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1639,7 +1639,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.04566893441758139</v>
+        <v>4.566893441758139</v>
       </c>
       <c r="F50" t="n">
         <v>2</v>
@@ -1663,7 +1663,7 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.0406139400796415</v>
+        <v>4.061394007964149</v>
       </c>
       <c r="F51" t="n">
         <v>1</v>
@@ -1687,7 +1687,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>0.04168313945362261</v>
+        <v>4.168313945362261</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -1711,7 +1711,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0.04190064278716337</v>
+        <v>4.190064278716337</v>
       </c>
       <c r="F53" t="n">
         <v>0</v>
@@ -1735,7 +1735,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>0.04404569058495775</v>
+        <v>4.404569058495776</v>
       </c>
       <c r="F54" t="n">
         <v>1</v>
@@ -1759,7 +1759,7 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>0.04202422037745236</v>
+        <v>4.202422037745236</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>0.04360089659942171</v>
+        <v>4.360089659942171</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>0.0461198645265793</v>
+        <v>4.61198645265793</v>
       </c>
       <c r="F57" t="n">
         <v>1</v>
@@ -1831,7 +1831,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>0.04525979251397377</v>
+        <v>4.525979251397377</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -1855,7 +1855,7 @@
         </is>
       </c>
       <c r="E59" t="n">
-        <v>0.04533955488460395</v>
+        <v>4.533955488460395</v>
       </c>
       <c r="F59" t="n">
         <v>0</v>
@@ -1879,7 +1879,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>0.04493698392003477</v>
+        <v>4.493698392003477</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
@@ -1903,7 +1903,7 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>0.0470760050705393</v>
+        <v>4.70760050705393</v>
       </c>
       <c r="F61" t="n">
         <v>1</v>
@@ -1927,7 +1927,7 @@
         </is>
       </c>
       <c r="E62" t="n">
-        <v>0.04675444377821496</v>
+        <v>4.675444377821496</v>
       </c>
       <c r="F62" t="n">
         <v>0</v>
@@ -1951,7 +1951,7 @@
         </is>
       </c>
       <c r="E63" t="n">
-        <v>0.04768196702476015</v>
+        <v>4.768196702476015</v>
       </c>
       <c r="F63" t="n">
         <v>0</v>
@@ -1975,7 +1975,7 @@
         </is>
       </c>
       <c r="E64" t="n">
-        <v>0.05478265863776734</v>
+        <v>5.478265863776734</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -1999,7 +1999,7 @@
         </is>
       </c>
       <c r="E65" t="n">
-        <v>0.04870111273685362</v>
+        <v>4.870111273685362</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="E66" t="n">
-        <v>0.0498060589848191</v>
+        <v>4.98060589848191</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -2047,7 +2047,7 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>0.05055391950638059</v>
+        <v>5.055391950638059</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
@@ -2071,7 +2071,7 @@
         </is>
       </c>
       <c r="E68" t="n">
-        <v>0.0494146064923221</v>
+        <v>4.94146064923221</v>
       </c>
       <c r="F68" t="n">
         <v>1</v>
@@ -2095,7 +2095,7 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>0.05156617215041128</v>
+        <v>5.156617215041128</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>0.05232712883936334</v>
+        <v>5.232712883936334</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
@@ -2143,7 +2143,7 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>0.0517377523216371</v>
+        <v>5.17377523216371</v>
       </c>
       <c r="F71" t="n">
         <v>0</v>
@@ -2167,7 +2167,7 @@
         </is>
       </c>
       <c r="E72" t="n">
-        <v>0.05447473306421173</v>
+        <v>5.447473306421173</v>
       </c>
       <c r="F72" t="n">
         <v>1</v>
@@ -2191,7 +2191,7 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>0.05430778065257086</v>
+        <v>5.430778065257086</v>
       </c>
       <c r="F73" t="n">
         <v>1</v>
@@ -2215,7 +2215,7 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>0.05298440415582022</v>
+        <v>5.298440415582022</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
@@ -2239,7 +2239,7 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>0.05498841790448361</v>
+        <v>5.498841790448362</v>
       </c>
       <c r="F75" t="n">
         <v>1</v>
@@ -2263,7 +2263,7 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>0.05456516886181714</v>
+        <v>5.456516886181713</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
@@ -2287,7 +2287,7 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>0.05511457064105142</v>
+        <v>5.511457064105143</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
@@ -2311,7 +2311,7 @@
         </is>
       </c>
       <c r="E78" t="n">
-        <v>0.05700513325832074</v>
+        <v>5.700513325832074</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>0.06271278267907188</v>
+        <v>6.271278267907188</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
@@ -2359,7 +2359,7 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>0.0600418207750139</v>
+        <v>6.00418207750139</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
@@ -2383,7 +2383,7 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>0.06110100405305822</v>
+        <v>6.110100405305822</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>0.05697994230898236</v>
+        <v>5.697994230898236</v>
       </c>
       <c r="F82" t="n">
         <v>1</v>
@@ -2431,7 +2431,7 @@
         </is>
       </c>
       <c r="E83" t="n">
-        <v>0.05892284635668621</v>
+        <v>5.892284635668621</v>
       </c>
       <c r="F83" t="n">
         <v>0</v>
@@ -2455,7 +2455,7 @@
         </is>
       </c>
       <c r="E84" t="n">
-        <v>0.06263173074789785</v>
+        <v>6.263173074789785</v>
       </c>
       <c r="F84" t="n">
         <v>1</v>
@@ -2479,7 +2479,7 @@
         </is>
       </c>
       <c r="E85" t="n">
-        <v>0.06161854985896797</v>
+        <v>6.161854985896797</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -2503,7 +2503,7 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>0.06006615982821659</v>
+        <v>6.006615982821659</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
@@ -2527,7 +2527,7 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>0.063686442038994</v>
+        <v>6.3686442038994</v>
       </c>
       <c r="F87" t="n">
         <v>1</v>
@@ -2551,7 +2551,7 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>0.06126447154283422</v>
+        <v>6.126447154283422</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -2575,7 +2575,7 @@
         </is>
       </c>
       <c r="E89" t="n">
-        <v>0.06346616566135997</v>
+        <v>6.346616566135997</v>
       </c>
       <c r="F89" t="n">
         <v>1</v>
@@ -2599,7 +2599,7 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>0.0641460765680152</v>
+        <v>6.41460765680152</v>
       </c>
       <c r="F90" t="n">
         <v>1</v>
@@ -2623,7 +2623,7 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>0.06432520104279006</v>
+        <v>6.432520104279006</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
@@ -2647,7 +2647,7 @@
         </is>
       </c>
       <c r="E92" t="n">
-        <v>0.06382918431828165</v>
+        <v>6.382918431828164</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
@@ -2671,7 +2671,7 @@
         </is>
       </c>
       <c r="E93" t="n">
-        <v>0.06360926905595708</v>
+        <v>6.360926905595708</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
@@ -2695,7 +2695,7 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>0.06253119034228183</v>
+        <v>6.253119034228183</v>
       </c>
       <c r="F94" t="n">
         <v>0</v>
@@ -2719,7 +2719,7 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>0.06588483811050005</v>
+        <v>6.588483811050006</v>
       </c>
       <c r="F95" t="n">
         <v>0</v>
@@ -2743,7 +2743,7 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>0.06331206976076305</v>
+        <v>6.331206976076305</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
@@ -2767,7 +2767,7 @@
         </is>
       </c>
       <c r="E97" t="n">
-        <v>0.06356740091679851</v>
+        <v>6.356740091679851</v>
       </c>
       <c r="F97" t="n">
         <v>0</v>
@@ -2791,7 +2791,7 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>0.06484027924687963</v>
+        <v>6.484027924687963</v>
       </c>
       <c r="F98" t="n">
         <v>0</v>
@@ -2815,7 +2815,7 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>0.06555838481125617</v>
+        <v>6.555838481125617</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
@@ -2839,7 +2839,7 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>0.06514673062498264</v>
+        <v>6.514673062498264</v>
       </c>
       <c r="F100" t="n">
         <v>1</v>
@@ -2863,7 +2863,7 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>0.0656911727486619</v>
+        <v>6.569117274866191</v>
       </c>
       <c r="F101" t="n">
         <v>0</v>
@@ -2887,7 +2887,7 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>0.06532126745148288</v>
+        <v>6.532126745148288</v>
       </c>
       <c r="F102" t="n">
         <v>0</v>
@@ -2911,7 +2911,7 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>0.07528076474531446</v>
+        <v>7.528076474531447</v>
       </c>
       <c r="F103" t="n">
         <v>0</v>
@@ -2935,7 +2935,7 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>0.06662287882204163</v>
+        <v>6.662287882204162</v>
       </c>
       <c r="F104" t="n">
         <v>0</v>
@@ -2959,7 +2959,7 @@
         </is>
       </c>
       <c r="E105" t="n">
-        <v>0.07105303455668419</v>
+        <v>7.105303455668419</v>
       </c>
       <c r="F105" t="n">
         <v>0</v>
@@ -2983,7 +2983,7 @@
         </is>
       </c>
       <c r="E106" t="n">
-        <v>0.06483997584541062</v>
+        <v>6.483997584541062</v>
       </c>
       <c r="F106" t="n">
         <v>0</v>
@@ -3007,7 +3007,7 @@
         </is>
       </c>
       <c r="E107" t="n">
-        <v>0.06783030911868734</v>
+        <v>6.783030911868734</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -3031,7 +3031,7 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>0.06919303862414317</v>
+        <v>6.919303862414317</v>
       </c>
       <c r="F108" t="n">
         <v>0</v>
@@ -3055,7 +3055,7 @@
         </is>
       </c>
       <c r="E109" t="n">
-        <v>0.07153624328221261</v>
+        <v>7.153624328221261</v>
       </c>
       <c r="F109" t="n">
         <v>0</v>
@@ -3079,7 +3079,7 @@
         </is>
       </c>
       <c r="E110" t="n">
-        <v>0.0662123253807451</v>
+        <v>6.62123253807451</v>
       </c>
       <c r="F110" t="n">
         <v>0</v>
@@ -3103,7 +3103,7 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>0.06632513868259117</v>
+        <v>6.632513868259117</v>
       </c>
       <c r="F111" t="n">
         <v>0</v>
@@ -3127,7 +3127,7 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>0.07097579068042349</v>
+        <v>7.097579068042349</v>
       </c>
       <c r="F112" t="n">
         <v>0</v>
@@ -3151,7 +3151,7 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>0.07371363362439255</v>
+        <v>7.371363362439255</v>
       </c>
       <c r="F113" t="n">
         <v>1</v>
@@ -3175,7 +3175,7 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>0.07338587138478972</v>
+        <v>7.338587138478972</v>
       </c>
       <c r="F114" t="n">
         <v>1</v>
@@ -3199,7 +3199,7 @@
         </is>
       </c>
       <c r="E115" t="n">
-        <v>0.06827472998546678</v>
+        <v>6.827472998546678</v>
       </c>
       <c r="F115" t="n">
         <v>0</v>
@@ -3223,7 +3223,7 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>0.06922870759872753</v>
+        <v>6.922870759872753</v>
       </c>
       <c r="F116" t="n">
         <v>0</v>
@@ -3247,7 +3247,7 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>0.06722041763341068</v>
+        <v>6.722041763341068</v>
       </c>
       <c r="F117" t="n">
         <v>0</v>
@@ -3271,7 +3271,7 @@
         </is>
       </c>
       <c r="E118" t="n">
-        <v>0.07342490608171763</v>
+        <v>7.342490608171763</v>
       </c>
       <c r="F118" t="n">
         <v>0</v>
@@ -3295,7 +3295,7 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>0.07185550254286163</v>
+        <v>7.185550254286163</v>
       </c>
       <c r="F119" t="n">
         <v>0</v>
@@ -3319,7 +3319,7 @@
         </is>
       </c>
       <c r="E120" t="n">
-        <v>0.07028123237261275</v>
+        <v>7.028123237261275</v>
       </c>
       <c r="F120" t="n">
         <v>0</v>
@@ -3343,7 +3343,7 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>0.07247855704790535</v>
+        <v>7.247855704790535</v>
       </c>
       <c r="F121" t="n">
         <v>1</v>
@@ -3367,7 +3367,7 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>0.06910898214366032</v>
+        <v>6.910898214366032</v>
       </c>
       <c r="F122" t="n">
         <v>0</v>
@@ -3391,7 +3391,7 @@
         </is>
       </c>
       <c r="E123" t="n">
-        <v>0.07376498414234263</v>
+        <v>7.376498414234263</v>
       </c>
       <c r="F123" t="n">
         <v>0</v>
@@ -3415,7 +3415,7 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>0.07159580092138056</v>
+        <v>7.159580092138055</v>
       </c>
       <c r="F124" t="n">
         <v>0</v>
@@ -3439,7 +3439,7 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>0.07161074623709909</v>
+        <v>7.16107462370991</v>
       </c>
       <c r="F125" t="n">
         <v>0</v>
@@ -3463,7 +3463,7 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>0.07117355158858027</v>
+        <v>7.117355158858027</v>
       </c>
       <c r="F126" t="n">
         <v>0</v>
@@ -3487,7 +3487,7 @@
         </is>
       </c>
       <c r="E127" t="n">
-        <v>0.07224308637760328</v>
+        <v>7.224308637760328</v>
       </c>
       <c r="F127" t="n">
         <v>0</v>
@@ -3511,7 +3511,7 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>0.07394770170602696</v>
+        <v>7.394770170602697</v>
       </c>
       <c r="F128" t="n">
         <v>0</v>
@@ -3535,7 +3535,7 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>0.07577287158553893</v>
+        <v>7.577287158553893</v>
       </c>
       <c r="F129" t="n">
         <v>1</v>
@@ -3559,7 +3559,7 @@
         </is>
       </c>
       <c r="E130" t="n">
-        <v>0.07270721981844405</v>
+        <v>7.270721981844405</v>
       </c>
       <c r="F130" t="n">
         <v>0</v>
@@ -3583,7 +3583,7 @@
         </is>
       </c>
       <c r="E131" t="n">
-        <v>0.07498681238418568</v>
+        <v>7.498681238418568</v>
       </c>
       <c r="F131" t="n">
         <v>0</v>
@@ -3607,7 +3607,7 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>0.07278623801466441</v>
+        <v>7.278623801466441</v>
       </c>
       <c r="F132" t="n">
         <v>1</v>
@@ -3631,7 +3631,7 @@
         </is>
       </c>
       <c r="E133" t="n">
-        <v>0.07495277889073322</v>
+        <v>7.495277889073322</v>
       </c>
       <c r="F133" t="n">
         <v>0</v>
@@ -3655,7 +3655,7 @@
         </is>
       </c>
       <c r="E134" t="n">
-        <v>0.07443050857604694</v>
+        <v>7.443050857604694</v>
       </c>
       <c r="F134" t="n">
         <v>0</v>
@@ -3679,7 +3679,7 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>0.07256770089384323</v>
+        <v>7.256770089384323</v>
       </c>
       <c r="F135" t="n">
         <v>0</v>
@@ -3703,7 +3703,7 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>0.0738510635095061</v>
+        <v>7.385106350950609</v>
       </c>
       <c r="F136" t="n">
         <v>0</v>
@@ -3727,7 +3727,7 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>0.07587567055853582</v>
+        <v>7.587567055853582</v>
       </c>
       <c r="F137" t="n">
         <v>0</v>
@@ -3751,7 +3751,7 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>0.07708496085965276</v>
+        <v>7.708496085965276</v>
       </c>
       <c r="F138" t="n">
         <v>0</v>
@@ -3775,7 +3775,7 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>0.07490346268278787</v>
+        <v>7.490346268278787</v>
       </c>
       <c r="F139" t="n">
         <v>1</v>
@@ -3799,7 +3799,7 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>0.07583873696081195</v>
+        <v>7.583873696081195</v>
       </c>
       <c r="F140" t="n">
         <v>1</v>
@@ -3823,7 +3823,7 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>0.07594599543857897</v>
+        <v>7.594599543857897</v>
       </c>
       <c r="F141" t="n">
         <v>0</v>
@@ -3847,7 +3847,7 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>0.07802741075669875</v>
+        <v>7.802741075669875</v>
       </c>
       <c r="F142" t="n">
         <v>0</v>
@@ -3871,7 +3871,7 @@
         </is>
       </c>
       <c r="E143" t="n">
-        <v>0.07776082927389329</v>
+        <v>7.776082927389329</v>
       </c>
       <c r="F143" t="n">
         <v>1</v>
@@ -3895,7 +3895,7 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>0.07650395105786388</v>
+        <v>7.650395105786388</v>
       </c>
       <c r="F144" t="n">
         <v>0</v>
@@ -3919,7 +3919,7 @@
         </is>
       </c>
       <c r="E145" t="n">
-        <v>0.07585269050141522</v>
+        <v>7.585269050141521</v>
       </c>
       <c r="F145" t="n">
         <v>0</v>
@@ -3943,7 +3943,7 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>0.07784196612160971</v>
+        <v>7.78419661216097</v>
       </c>
       <c r="F146" t="n">
         <v>0</v>
@@ -3967,7 +3967,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>0.0757591967110391</v>
+        <v>7.57591967110391</v>
       </c>
       <c r="F147" t="n">
         <v>0</v>
@@ -3991,7 +3991,7 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>0.07606886016854608</v>
+        <v>7.606886016854608</v>
       </c>
       <c r="F148" t="n">
         <v>0</v>
@@ -4015,7 +4015,7 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>0.07629807183897917</v>
+        <v>7.629807183897917</v>
       </c>
       <c r="F149" t="n">
         <v>0</v>
@@ -4039,7 +4039,7 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>0.07777283764834639</v>
+        <v>7.777283764834639</v>
       </c>
       <c r="F150" t="n">
         <v>1</v>
@@ -4063,7 +4063,7 @@
         </is>
       </c>
       <c r="E151" t="n">
-        <v>0.07526571849943212</v>
+        <v>7.526571849943211</v>
       </c>
       <c r="F151" t="n">
         <v>1</v>
@@ -4087,7 +4087,7 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>0.07549241306983909</v>
+        <v>7.549241306983909</v>
       </c>
       <c r="F152" t="n">
         <v>1</v>
@@ -4111,7 +4111,7 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>0.07772409196934356</v>
+        <v>7.772409196934356</v>
       </c>
       <c r="F153" t="n">
         <v>0</v>
@@ -4135,7 +4135,7 @@
         </is>
       </c>
       <c r="E154" t="n">
-        <v>0.07808436867957237</v>
+        <v>7.808436867957237</v>
       </c>
       <c r="F154" t="n">
         <v>0</v>
@@ -4159,7 +4159,7 @@
         </is>
       </c>
       <c r="E155" t="n">
-        <v>0.0786596866700027</v>
+        <v>7.86596866700027</v>
       </c>
       <c r="F155" t="n">
         <v>1</v>
@@ -4183,7 +4183,7 @@
         </is>
       </c>
       <c r="E156" t="n">
-        <v>0.07626490720485499</v>
+        <v>7.626490720485498</v>
       </c>
       <c r="F156" t="n">
         <v>0</v>
@@ -4207,7 +4207,7 @@
         </is>
       </c>
       <c r="E157" t="n">
-        <v>0.07698598565109104</v>
+        <v>7.698598565109103</v>
       </c>
       <c r="F157" t="n">
         <v>1</v>
@@ -4231,7 +4231,7 @@
         </is>
       </c>
       <c r="E158" t="n">
-        <v>0.0794090181430096</v>
+        <v>7.94090181430096</v>
       </c>
       <c r="F158" t="n">
         <v>0</v>
@@ -4255,7 +4255,7 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>0.07842611941631392</v>
+        <v>7.842611941631391</v>
       </c>
       <c r="F159" t="n">
         <v>0</v>
@@ -4279,7 +4279,7 @@
         </is>
       </c>
       <c r="E160" t="n">
-        <v>0.0769605090772974</v>
+        <v>7.69605090772974</v>
       </c>
       <c r="F160" t="n">
         <v>0</v>
@@ -4303,7 +4303,7 @@
         </is>
       </c>
       <c r="E161" t="n">
-        <v>0.07776456599286563</v>
+        <v>7.776456599286563</v>
       </c>
       <c r="F161" t="n">
         <v>0</v>
@@ -4327,7 +4327,7 @@
         </is>
       </c>
       <c r="E162" t="n">
-        <v>0.08687639021290118</v>
+        <v>8.687639021290119</v>
       </c>
       <c r="F162" t="n">
         <v>2</v>
@@ -4351,7 +4351,7 @@
         </is>
       </c>
       <c r="E163" t="n">
-        <v>0.07946314059141242</v>
+        <v>7.946314059141242</v>
       </c>
       <c r="F163" t="n">
         <v>0</v>
@@ -4375,7 +4375,7 @@
         </is>
       </c>
       <c r="E164" t="n">
-        <v>0.07824261152048173</v>
+        <v>7.824261152048173</v>
       </c>
       <c r="F164" t="n">
         <v>0</v>
@@ -4399,7 +4399,7 @@
         </is>
       </c>
       <c r="E165" t="n">
-        <v>0.0786247234824341</v>
+        <v>7.86247234824341</v>
       </c>
       <c r="F165" t="n">
         <v>0</v>
@@ -4423,7 +4423,7 @@
         </is>
       </c>
       <c r="E166" t="n">
-        <v>0.0810368349249659</v>
+        <v>8.103683492496589</v>
       </c>
       <c r="F166" t="n">
         <v>0</v>
@@ -4447,7 +4447,7 @@
         </is>
       </c>
       <c r="E167" t="n">
-        <v>0.0775357270621905</v>
+        <v>7.75357270621905</v>
       </c>
       <c r="F167" t="n">
         <v>0</v>
@@ -4471,7 +4471,7 @@
         </is>
       </c>
       <c r="E168" t="n">
-        <v>0.07884702767844795</v>
+        <v>7.884702767844795</v>
       </c>
       <c r="F168" t="n">
         <v>0</v>
@@ -4495,7 +4495,7 @@
         </is>
       </c>
       <c r="E169" t="n">
-        <v>0.07962854477207143</v>
+        <v>7.962854477207143</v>
       </c>
       <c r="F169" t="n">
         <v>0</v>
@@ -4519,7 +4519,7 @@
         </is>
       </c>
       <c r="E170" t="n">
-        <v>0.07837462834489593</v>
+        <v>7.837462834489593</v>
       </c>
       <c r="F170" t="n">
         <v>0</v>
@@ -4543,7 +4543,7 @@
         </is>
       </c>
       <c r="E171" t="n">
-        <v>0.08019005543283457</v>
+        <v>8.019005543283457</v>
       </c>
       <c r="F171" t="n">
         <v>1</v>
@@ -4567,7 +4567,7 @@
         </is>
       </c>
       <c r="E172" t="n">
-        <v>0.08124788637132228</v>
+        <v>8.124788637132228</v>
       </c>
       <c r="F172" t="n">
         <v>1</v>
@@ -4591,7 +4591,7 @@
         </is>
       </c>
       <c r="E173" t="n">
-        <v>0.08669076569175156</v>
+        <v>8.669076569175155</v>
       </c>
       <c r="F173" t="n">
         <v>0</v>
@@ -4615,7 +4615,7 @@
         </is>
       </c>
       <c r="E174" t="n">
-        <v>0.08499954763412648</v>
+        <v>8.499954763412648</v>
       </c>
       <c r="F174" t="n">
         <v>1</v>
@@ -4639,7 +4639,7 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>0.08025736539112767</v>
+        <v>8.025736539112767</v>
       </c>
       <c r="F175" t="n">
         <v>0</v>
@@ -4663,7 +4663,7 @@
         </is>
       </c>
       <c r="E176" t="n">
-        <v>0.08416137914521729</v>
+        <v>8.416137914521729</v>
       </c>
       <c r="F176" t="n">
         <v>1</v>
@@ -4687,7 +4687,7 @@
         </is>
       </c>
       <c r="E177" t="n">
-        <v>0.08548634095736798</v>
+        <v>8.548634095736798</v>
       </c>
       <c r="F177" t="n">
         <v>1</v>
@@ -4711,7 +4711,7 @@
         </is>
       </c>
       <c r="E178" t="n">
-        <v>0.08420682377769961</v>
+        <v>8.42068237776996</v>
       </c>
       <c r="F178" t="n">
         <v>1</v>
@@ -4735,7 +4735,7 @@
         </is>
       </c>
       <c r="E179" t="n">
-        <v>0.08084705460092423</v>
+        <v>8.084705460092422</v>
       </c>
       <c r="F179" t="n">
         <v>0</v>
@@ -4759,7 +4759,7 @@
         </is>
       </c>
       <c r="E180" t="n">
-        <v>0.08552298073673538</v>
+        <v>8.552298073673539</v>
       </c>
       <c r="F180" t="n">
         <v>2</v>
@@ -4783,7 +4783,7 @@
         </is>
       </c>
       <c r="E181" t="n">
-        <v>0.08457161287349967</v>
+        <v>8.457161287349967</v>
       </c>
       <c r="F181" t="n">
         <v>1</v>
@@ -4807,7 +4807,7 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>0.08139045928140914</v>
+        <v>8.139045928140915</v>
       </c>
       <c r="F182" t="n">
         <v>0</v>
@@ -4831,7 +4831,7 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>0.0835138234169958</v>
+        <v>8.35138234169958</v>
       </c>
       <c r="F183" t="n">
         <v>0</v>
@@ -4855,7 +4855,7 @@
         </is>
       </c>
       <c r="E184" t="n">
-        <v>0.08361852339356228</v>
+        <v>8.361852339356227</v>
       </c>
       <c r="F184" t="n">
         <v>0</v>
@@ -4879,7 +4879,7 @@
         </is>
       </c>
       <c r="E185" t="n">
-        <v>0.0845973609569614</v>
+        <v>8.45973609569614</v>
       </c>
       <c r="F185" t="n">
         <v>2</v>
@@ -4903,7 +4903,7 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>0.08249840119377531</v>
+        <v>8.249840119377531</v>
       </c>
       <c r="F186" t="n">
         <v>0</v>
@@ -4927,7 +4927,7 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>0.08059075379492281</v>
+        <v>8.059075379492281</v>
       </c>
       <c r="F187" t="n">
         <v>0</v>
@@ -4951,7 +4951,7 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>0.08355323189227848</v>
+        <v>8.355323189227848</v>
       </c>
       <c r="F188" t="n">
         <v>0</v>
@@ -4975,7 +4975,7 @@
         </is>
       </c>
       <c r="E189" t="n">
-        <v>0.08546158943773258</v>
+        <v>8.546158943773257</v>
       </c>
       <c r="F189" t="n">
         <v>1</v>
@@ -4999,7 +4999,7 @@
         </is>
       </c>
       <c r="E190" t="n">
-        <v>0.0846036781964972</v>
+        <v>8.46036781964972</v>
       </c>
       <c r="F190" t="n">
         <v>1</v>
@@ -5023,7 +5023,7 @@
         </is>
       </c>
       <c r="E191" t="n">
-        <v>0.08444623968089672</v>
+        <v>8.444623968089672</v>
       </c>
       <c r="F191" t="n">
         <v>0</v>
@@ -5047,7 +5047,7 @@
         </is>
       </c>
       <c r="E192" t="n">
-        <v>0.0833372480856861</v>
+        <v>8.33372480856861</v>
       </c>
       <c r="F192" t="n">
         <v>0</v>
@@ -5071,7 +5071,7 @@
         </is>
       </c>
       <c r="E193" t="n">
-        <v>0.08465475080041344</v>
+        <v>8.465475080041344</v>
       </c>
       <c r="F193" t="n">
         <v>0</v>
@@ -5095,7 +5095,7 @@
         </is>
       </c>
       <c r="E194" t="n">
-        <v>0.08724577976655538</v>
+        <v>8.724577976655539</v>
       </c>
       <c r="F194" t="n">
         <v>1</v>
@@ -5119,7 +5119,7 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>0.08614337614491122</v>
+        <v>8.614337614491122</v>
       </c>
       <c r="F195" t="n">
         <v>0</v>
@@ -5143,7 +5143,7 @@
         </is>
       </c>
       <c r="E196" t="n">
-        <v>0.08503677579526207</v>
+        <v>8.503677579526208</v>
       </c>
       <c r="F196" t="n">
         <v>1</v>
@@ -5167,7 +5167,7 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>0.08460931763170061</v>
+        <v>8.460931763170061</v>
       </c>
       <c r="F197" t="n">
         <v>0</v>
@@ -5191,7 +5191,7 @@
         </is>
       </c>
       <c r="E198" t="n">
-        <v>0.0854243588777535</v>
+        <v>8.542435887775349</v>
       </c>
       <c r="F198" t="n">
         <v>0</v>
@@ -5215,7 +5215,7 @@
         </is>
       </c>
       <c r="E199" t="n">
-        <v>0.08511777301927195</v>
+        <v>8.511777301927195</v>
       </c>
       <c r="F199" t="n">
         <v>1</v>
@@ -5239,7 +5239,7 @@
         </is>
       </c>
       <c r="E200" t="n">
-        <v>0.08953052002757142</v>
+        <v>8.953052002757142</v>
       </c>
       <c r="F200" t="n">
         <v>1</v>
@@ -5263,7 +5263,7 @@
         </is>
       </c>
       <c r="E201" t="n">
-        <v>0.08558253438932889</v>
+        <v>8.558253438932889</v>
       </c>
       <c r="F201" t="n">
         <v>2</v>
@@ -5287,7 +5287,7 @@
         </is>
       </c>
       <c r="E202" t="n">
-        <v>0.08585485854858549</v>
+        <v>8.585485854858549</v>
       </c>
       <c r="F202" t="n">
         <v>0</v>
@@ -5311,7 +5311,7 @@
         </is>
       </c>
       <c r="E203" t="n">
-        <v>0.08502024291497975</v>
+        <v>8.502024291497975</v>
       </c>
       <c r="F203" t="n">
         <v>0</v>
@@ -5335,7 +5335,7 @@
         </is>
       </c>
       <c r="E204" t="n">
-        <v>0.08489277969640993</v>
+        <v>8.489277969640993</v>
       </c>
       <c r="F204" t="n">
         <v>1</v>
@@ -5359,7 +5359,7 @@
         </is>
       </c>
       <c r="E205" t="n">
-        <v>0.0858343949044586</v>
+        <v>8.58343949044586</v>
       </c>
       <c r="F205" t="n">
         <v>0</v>
@@ -5383,7 +5383,7 @@
         </is>
       </c>
       <c r="E206" t="n">
-        <v>0.09009328459985816</v>
+        <v>9.009328459985817</v>
       </c>
       <c r="F206" t="n">
         <v>0</v>
@@ -5407,7 +5407,7 @@
         </is>
       </c>
       <c r="E207" t="n">
-        <v>0.09682316881033544</v>
+        <v>9.682316881033543</v>
       </c>
       <c r="F207" t="n">
         <v>1</v>
@@ -5431,7 +5431,7 @@
         </is>
       </c>
       <c r="E208" t="n">
-        <v>0.08668351528099841</v>
+        <v>8.668351528099841</v>
       </c>
       <c r="F208" t="n">
         <v>0</v>
@@ -5455,7 +5455,7 @@
         </is>
       </c>
       <c r="E209" t="n">
-        <v>0.08960756399580971</v>
+        <v>8.960756399580971</v>
       </c>
       <c r="F209" t="n">
         <v>0</v>
@@ -5479,7 +5479,7 @@
         </is>
       </c>
       <c r="E210" t="n">
-        <v>0.09178045515394913</v>
+        <v>9.178045515394913</v>
       </c>
       <c r="F210" t="n">
         <v>1</v>
@@ -5503,7 +5503,7 @@
         </is>
       </c>
       <c r="E211" t="n">
-        <v>0.0874076362606524</v>
+        <v>8.74076362606524</v>
       </c>
       <c r="F211" t="n">
         <v>0</v>
@@ -5527,7 +5527,7 @@
         </is>
       </c>
       <c r="E212" t="n">
-        <v>0.08806559368357121</v>
+        <v>8.806559368357121</v>
       </c>
       <c r="F212" t="n">
         <v>0</v>
@@ -5551,7 +5551,7 @@
         </is>
       </c>
       <c r="E213" t="n">
-        <v>0.08973420430228629</v>
+        <v>8.973420430228629</v>
       </c>
       <c r="F213" t="n">
         <v>0</v>
@@ -5575,7 +5575,7 @@
         </is>
       </c>
       <c r="E214" t="n">
-        <v>0.08334483615382492</v>
+        <v>8.334483615382492</v>
       </c>
       <c r="F214" t="n">
         <v>1</v>
@@ -5599,7 +5599,7 @@
         </is>
       </c>
       <c r="E215" t="n">
-        <v>0.08795878259945822</v>
+        <v>8.795878259945821</v>
       </c>
       <c r="F215" t="n">
         <v>0</v>
@@ -5623,7 +5623,7 @@
         </is>
       </c>
       <c r="E216" t="n">
-        <v>0.08694136886410551</v>
+        <v>8.694136886410551</v>
       </c>
       <c r="F216" t="n">
         <v>0</v>
@@ -5647,7 +5647,7 @@
         </is>
       </c>
       <c r="E217" t="n">
-        <v>0.08994678051348032</v>
+        <v>8.994678051348032</v>
       </c>
       <c r="F217" t="n">
         <v>1</v>
@@ -5671,7 +5671,7 @@
         </is>
       </c>
       <c r="E218" t="n">
-        <v>0.09028801451411725</v>
+        <v>9.028801451411725</v>
       </c>
       <c r="F218" t="n">
         <v>0</v>
@@ -5695,7 +5695,7 @@
         </is>
       </c>
       <c r="E219" t="n">
-        <v>0.09376974598761531</v>
+        <v>9.376974598761532</v>
       </c>
       <c r="F219" t="n">
         <v>1</v>
@@ -5719,7 +5719,7 @@
         </is>
       </c>
       <c r="E220" t="n">
-        <v>0.08989145183175033</v>
+        <v>8.989145183175033</v>
       </c>
       <c r="F220" t="n">
         <v>0</v>
@@ -5743,7 +5743,7 @@
         </is>
       </c>
       <c r="E221" t="n">
-        <v>0.08793619142572283</v>
+        <v>8.793619142572282</v>
       </c>
       <c r="F221" t="n">
         <v>0</v>
@@ -5767,7 +5767,7 @@
         </is>
       </c>
       <c r="E222" t="n">
-        <v>0.08859416445623342</v>
+        <v>8.859416445623342</v>
       </c>
       <c r="F222" t="n">
         <v>0</v>
@@ -5791,7 +5791,7 @@
         </is>
       </c>
       <c r="E223" t="n">
-        <v>0.09078939836281413</v>
+        <v>9.078939836281414</v>
       </c>
       <c r="F223" t="n">
         <v>0</v>
@@ -5815,7 +5815,7 @@
         </is>
       </c>
       <c r="E224" t="n">
-        <v>0.08794347122037391</v>
+        <v>8.79434712203739</v>
       </c>
       <c r="F224" t="n">
         <v>0</v>
@@ -5839,7 +5839,7 @@
         </is>
       </c>
       <c r="E225" t="n">
-        <v>0.08495228134396653</v>
+        <v>8.495228134396653</v>
       </c>
       <c r="F225" t="n">
         <v>1</v>
@@ -5863,7 +5863,7 @@
         </is>
       </c>
       <c r="E226" t="n">
-        <v>0.08945166633910773</v>
+        <v>8.945166633910773</v>
       </c>
       <c r="F226" t="n">
         <v>0</v>
@@ -5887,7 +5887,7 @@
         </is>
       </c>
       <c r="E227" t="n">
-        <v>0.08702073116362015</v>
+        <v>8.702073116362016</v>
       </c>
       <c r="F227" t="n">
         <v>0</v>
@@ -5911,7 +5911,7 @@
         </is>
       </c>
       <c r="E228" t="n">
-        <v>0.08742436436257414</v>
+        <v>8.742436436257414</v>
       </c>
       <c r="F228" t="n">
         <v>0</v>
@@ -5935,7 +5935,7 @@
         </is>
       </c>
       <c r="E229" t="n">
-        <v>0.08685459940652819</v>
+        <v>8.685459940652819</v>
       </c>
       <c r="F229" t="n">
         <v>1</v>
@@ -5959,7 +5959,7 @@
         </is>
       </c>
       <c r="E230" t="n">
-        <v>0.08642512997795139</v>
+        <v>8.642512997795139</v>
       </c>
       <c r="F230" t="n">
         <v>0</v>
@@ -5983,7 +5983,7 @@
         </is>
       </c>
       <c r="E231" t="n">
-        <v>0.08774052310173983</v>
+        <v>8.774052310173982</v>
       </c>
       <c r="F231" t="n">
         <v>0</v>
@@ -6007,7 +6007,7 @@
         </is>
       </c>
       <c r="E232" t="n">
-        <v>0.08911366473544381</v>
+        <v>8.911366473544382</v>
       </c>
       <c r="F232" t="n">
         <v>1</v>
@@ -6031,7 +6031,7 @@
         </is>
       </c>
       <c r="E233" t="n">
-        <v>0.09485668895214139</v>
+        <v>9.48566889521414</v>
       </c>
       <c r="F233" t="n">
         <v>0</v>
@@ -6055,7 +6055,7 @@
         </is>
       </c>
       <c r="E234" t="n">
-        <v>0.08961232169423296</v>
+        <v>8.961232169423296</v>
       </c>
       <c r="F234" t="n">
         <v>0</v>
@@ -6079,7 +6079,7 @@
         </is>
       </c>
       <c r="E235" t="n">
-        <v>0.0893939393939394</v>
+        <v>8.939393939393939</v>
       </c>
       <c r="F235" t="n">
         <v>0</v>
@@ -6103,7 +6103,7 @@
         </is>
       </c>
       <c r="E236" t="n">
-        <v>0.08957926604985429</v>
+        <v>8.957926604985429</v>
       </c>
       <c r="F236" t="n">
         <v>0</v>
@@ -6127,7 +6127,7 @@
         </is>
       </c>
       <c r="E237" t="n">
-        <v>0.09177820267686425</v>
+        <v>9.177820267686425</v>
       </c>
       <c r="F237" t="n">
         <v>0</v>
@@ -6151,7 +6151,7 @@
         </is>
       </c>
       <c r="E238" t="n">
-        <v>0.08814802373754339</v>
+        <v>8.81480237375434</v>
       </c>
       <c r="F238" t="n">
         <v>0</v>
@@ -6175,7 +6175,7 @@
         </is>
       </c>
       <c r="E239" t="n">
-        <v>0.09223814561892854</v>
+        <v>9.223814561892855</v>
       </c>
       <c r="F239" t="n">
         <v>1</v>
@@ -6199,7 +6199,7 @@
         </is>
       </c>
       <c r="E240" t="n">
-        <v>0.09023049534636766</v>
+        <v>9.023049534636767</v>
       </c>
       <c r="F240" t="n">
         <v>0</v>
@@ -6223,7 +6223,7 @@
         </is>
       </c>
       <c r="E241" t="n">
-        <v>0.09073412152873248</v>
+        <v>9.073412152873248</v>
       </c>
       <c r="F241" t="n">
         <v>1</v>
@@ -6247,7 +6247,7 @@
         </is>
       </c>
       <c r="E242" t="n">
-        <v>0.09231991201808518</v>
+        <v>9.231991201808517</v>
       </c>
       <c r="F242" t="n">
         <v>1</v>
@@ -6271,7 +6271,7 @@
         </is>
       </c>
       <c r="E243" t="n">
-        <v>0.09270134228187919</v>
+        <v>9.270134228187919</v>
       </c>
       <c r="F243" t="n">
         <v>1</v>
@@ -6295,7 +6295,7 @@
         </is>
       </c>
       <c r="E244" t="n">
-        <v>0.09389274763781991</v>
+        <v>9.389274763781991</v>
       </c>
       <c r="F244" t="n">
         <v>1</v>
@@ -6319,7 +6319,7 @@
         </is>
       </c>
       <c r="E245" t="n">
-        <v>0.09042024120353102</v>
+        <v>9.042024120353103</v>
       </c>
       <c r="F245" t="n">
         <v>1</v>
@@ -6343,7 +6343,7 @@
         </is>
       </c>
       <c r="E246" t="n">
-        <v>0.09498238533365257</v>
+        <v>9.498238533365257</v>
       </c>
       <c r="F246" t="n">
         <v>0</v>
@@ -6367,7 +6367,7 @@
         </is>
       </c>
       <c r="E247" t="n">
-        <v>0.09592283142682971</v>
+        <v>9.592283142682971</v>
       </c>
       <c r="F247" t="n">
         <v>1</v>
@@ -6391,7 +6391,7 @@
         </is>
       </c>
       <c r="E248" t="n">
-        <v>0.09891240951041273</v>
+        <v>9.891240951041274</v>
       </c>
       <c r="F248" t="n">
         <v>1</v>
@@ -6415,7 +6415,7 @@
         </is>
       </c>
       <c r="E249" t="n">
-        <v>0.09173814286198596</v>
+        <v>9.173814286198596</v>
       </c>
       <c r="F249" t="n">
         <v>1</v>
@@ -6439,7 +6439,7 @@
         </is>
       </c>
       <c r="E250" t="n">
-        <v>0.09140688196129675</v>
+        <v>9.140688196129675</v>
       </c>
       <c r="F250" t="n">
         <v>0</v>
@@ -6463,7 +6463,7 @@
         </is>
       </c>
       <c r="E251" t="n">
-        <v>0.09030110364683301</v>
+        <v>9.030110364683301</v>
       </c>
       <c r="F251" t="n">
         <v>0</v>
@@ -6487,7 +6487,7 @@
         </is>
       </c>
       <c r="E252" t="n">
-        <v>0.1106971508215176</v>
+        <v>11.06971508215176</v>
       </c>
       <c r="F252" t="n">
         <v>1</v>
@@ -6511,7 +6511,7 @@
         </is>
       </c>
       <c r="E253" t="n">
-        <v>0.09195643066610809</v>
+        <v>9.19564306661081</v>
       </c>
       <c r="F253" t="n">
         <v>0</v>
@@ -6535,7 +6535,7 @@
         </is>
       </c>
       <c r="E254" t="n">
-        <v>0.09177693190743762</v>
+        <v>9.177693190743762</v>
       </c>
       <c r="F254" t="n">
         <v>0</v>
@@ -6559,7 +6559,7 @@
         </is>
       </c>
       <c r="E255" t="n">
-        <v>0.0978601997146933</v>
+        <v>9.786019971469329</v>
       </c>
       <c r="F255" t="n">
         <v>0</v>
@@ -6583,7 +6583,7 @@
         </is>
       </c>
       <c r="E256" t="n">
-        <v>0.09089746459059372</v>
+        <v>9.089746459059372</v>
       </c>
       <c r="F256" t="n">
         <v>0</v>
@@ -6607,7 +6607,7 @@
         </is>
       </c>
       <c r="E257" t="n">
-        <v>0.09069301976482362</v>
+        <v>9.069301976482363</v>
       </c>
       <c r="F257" t="n">
         <v>0</v>
@@ -6631,7 +6631,7 @@
         </is>
       </c>
       <c r="E258" t="n">
-        <v>0.09052387171673197</v>
+        <v>9.052387171673198</v>
       </c>
       <c r="F258" t="n">
         <v>0</v>
@@ -6655,7 +6655,7 @@
         </is>
       </c>
       <c r="E259" t="n">
-        <v>0.09181503697356311</v>
+        <v>9.181503697356311</v>
       </c>
       <c r="F259" t="n">
         <v>0</v>
@@ -6679,7 +6679,7 @@
         </is>
       </c>
       <c r="E260" t="n">
-        <v>0.0938768038563627</v>
+        <v>9.387680385636269</v>
       </c>
       <c r="F260" t="n">
         <v>0</v>
@@ -6703,7 +6703,7 @@
         </is>
       </c>
       <c r="E261" t="n">
-        <v>0.09232944747189073</v>
+        <v>9.232944747189073</v>
       </c>
       <c r="F261" t="n">
         <v>0</v>
@@ -6727,7 +6727,7 @@
         </is>
       </c>
       <c r="E262" t="n">
-        <v>0.09096070144452154</v>
+        <v>9.096070144452154</v>
       </c>
       <c r="F262" t="n">
         <v>0</v>
@@ -6751,7 +6751,7 @@
         </is>
       </c>
       <c r="E263" t="n">
-        <v>0.09320639018880103</v>
+        <v>9.320639018880103</v>
       </c>
       <c r="F263" t="n">
         <v>1</v>
@@ -6775,7 +6775,7 @@
         </is>
       </c>
       <c r="E264" t="n">
-        <v>0.09590177005262318</v>
+        <v>9.590177005262317</v>
       </c>
       <c r="F264" t="n">
         <v>1</v>
@@ -6799,7 +6799,7 @@
         </is>
       </c>
       <c r="E265" t="n">
-        <v>0.09282409685992715</v>
+        <v>9.282409685992715</v>
       </c>
       <c r="F265" t="n">
         <v>0</v>
@@ -6823,7 +6823,7 @@
         </is>
       </c>
       <c r="E266" t="n">
-        <v>0.09156711398648432</v>
+        <v>9.156711398648431</v>
       </c>
       <c r="F266" t="n">
         <v>0</v>
@@ -6847,7 +6847,7 @@
         </is>
       </c>
       <c r="E267" t="n">
-        <v>0.09559605701723282</v>
+        <v>9.559605701723282</v>
       </c>
       <c r="F267" t="n">
         <v>1</v>
@@ -6871,7 +6871,7 @@
         </is>
       </c>
       <c r="E268" t="n">
-        <v>0.09222946024993353</v>
+        <v>9.222946024993353</v>
       </c>
       <c r="F268" t="n">
         <v>0</v>
@@ -6895,7 +6895,7 @@
         </is>
       </c>
       <c r="E269" t="n">
-        <v>0.09195366699702676</v>
+        <v>9.195366699702676</v>
       </c>
       <c r="F269" t="n">
         <v>0</v>
@@ -6919,7 +6919,7 @@
         </is>
       </c>
       <c r="E270" t="n">
-        <v>0.0955831823577185</v>
+        <v>9.55831823577185</v>
       </c>
       <c r="F270" t="n">
         <v>0</v>
@@ -6943,7 +6943,7 @@
         </is>
       </c>
       <c r="E271" t="n">
-        <v>0.09184551995572228</v>
+        <v>9.184551995572228</v>
       </c>
       <c r="F271" t="n">
         <v>0</v>
@@ -6967,7 +6967,7 @@
         </is>
       </c>
       <c r="E272" t="n">
-        <v>0.09784331289189004</v>
+        <v>9.784331289189003</v>
       </c>
       <c r="F272" t="n">
         <v>1</v>
@@ -6991,7 +6991,7 @@
         </is>
       </c>
       <c r="E273" t="n">
-        <v>0.09819736108530012</v>
+        <v>9.819736108530012</v>
       </c>
       <c r="F273" t="n">
         <v>0</v>
@@ -7015,7 +7015,7 @@
         </is>
       </c>
       <c r="E274" t="n">
-        <v>0.09391720642072655</v>
+        <v>9.391720642072656</v>
       </c>
       <c r="F274" t="n">
         <v>0</v>
@@ -7039,7 +7039,7 @@
         </is>
       </c>
       <c r="E275" t="n">
-        <v>0.09874246595728849</v>
+        <v>9.874246595728849</v>
       </c>
       <c r="F275" t="n">
         <v>0</v>
@@ -7063,7 +7063,7 @@
         </is>
       </c>
       <c r="E276" t="n">
-        <v>0.0963079615048119</v>
+        <v>9.63079615048119</v>
       </c>
       <c r="F276" t="n">
         <v>0</v>
@@ -7087,7 +7087,7 @@
         </is>
       </c>
       <c r="E277" t="n">
-        <v>0.1010943020822613</v>
+        <v>10.10943020822613</v>
       </c>
       <c r="F277" t="n">
         <v>1</v>
@@ -7111,7 +7111,7 @@
         </is>
       </c>
       <c r="E278" t="n">
-        <v>0.0984299738941795</v>
+        <v>9.842997389417949</v>
       </c>
       <c r="F278" t="n">
         <v>0</v>
@@ -7135,7 +7135,7 @@
         </is>
       </c>
       <c r="E279" t="n">
-        <v>0.0952051477201965</v>
+        <v>9.52051477201965</v>
       </c>
       <c r="F279" t="n">
         <v>1</v>
@@ -7159,7 +7159,7 @@
         </is>
       </c>
       <c r="E280" t="n">
-        <v>0.1027201263033253</v>
+        <v>10.27201263033253</v>
       </c>
       <c r="F280" t="n">
         <v>1</v>
@@ -7183,7 +7183,7 @@
         </is>
       </c>
       <c r="E281" t="n">
-        <v>0.09369972750254441</v>
+        <v>9.369972750254441</v>
       </c>
       <c r="F281" t="n">
         <v>0</v>
@@ -7207,7 +7207,7 @@
         </is>
       </c>
       <c r="E282" t="n">
-        <v>0.09482234801240845</v>
+        <v>9.482234801240844</v>
       </c>
       <c r="F282" t="n">
         <v>0</v>
@@ -7231,7 +7231,7 @@
         </is>
       </c>
       <c r="E283" t="n">
-        <v>0.0980357891793653</v>
+        <v>9.80357891793653</v>
       </c>
       <c r="F283" t="n">
         <v>0</v>
@@ -7255,7 +7255,7 @@
         </is>
       </c>
       <c r="E284" t="n">
-        <v>0.09865122519596074</v>
+        <v>9.865122519596074</v>
       </c>
       <c r="F284" t="n">
         <v>0</v>
@@ -7279,7 +7279,7 @@
         </is>
       </c>
       <c r="E285" t="n">
-        <v>0.09634320308966285</v>
+        <v>9.634320308966284</v>
       </c>
       <c r="F285" t="n">
         <v>0</v>
@@ -7303,7 +7303,7 @@
         </is>
       </c>
       <c r="E286" t="n">
-        <v>0.09756608583301324</v>
+        <v>9.756608583301324</v>
       </c>
       <c r="F286" t="n">
         <v>0</v>
@@ -7327,7 +7327,7 @@
         </is>
       </c>
       <c r="E287" t="n">
-        <v>0.09661669646541053</v>
+        <v>9.661669646541053</v>
       </c>
       <c r="F287" t="n">
         <v>0</v>
@@ -7351,7 +7351,7 @@
         </is>
       </c>
       <c r="E288" t="n">
-        <v>0.1031797534068787</v>
+        <v>10.31797534068787</v>
       </c>
       <c r="F288" t="n">
         <v>2</v>
@@ -7375,7 +7375,7 @@
         </is>
       </c>
       <c r="E289" t="n">
-        <v>0.09562303520226621</v>
+        <v>9.562303520226621</v>
       </c>
       <c r="F289" t="n">
         <v>0</v>
@@ -7399,7 +7399,7 @@
         </is>
       </c>
       <c r="E290" t="n">
-        <v>0.09729561703450419</v>
+        <v>9.72956170345042</v>
       </c>
       <c r="F290" t="n">
         <v>1</v>
@@ -7423,7 +7423,7 @@
         </is>
       </c>
       <c r="E291" t="n">
-        <v>0.09659714599341383</v>
+        <v>9.659714599341383</v>
       </c>
       <c r="F291" t="n">
         <v>0</v>
@@ -7447,7 +7447,7 @@
         </is>
       </c>
       <c r="E292" t="n">
-        <v>0.09471549132529247</v>
+        <v>9.471549132529248</v>
       </c>
       <c r="F292" t="n">
         <v>1</v>
@@ -7471,7 +7471,7 @@
         </is>
       </c>
       <c r="E293" t="n">
-        <v>0.094463357821179</v>
+        <v>9.446335782117901</v>
       </c>
       <c r="F293" t="n">
         <v>0</v>
@@ -7495,7 +7495,7 @@
         </is>
       </c>
       <c r="E294" t="n">
-        <v>0.1008109397360471</v>
+        <v>10.08109397360471</v>
       </c>
       <c r="F294" t="n">
         <v>1</v>
@@ -7519,7 +7519,7 @@
         </is>
       </c>
       <c r="E295" t="n">
-        <v>0.1011673151750973</v>
+        <v>10.11673151750973</v>
       </c>
       <c r="F295" t="n">
         <v>0</v>
@@ -7543,7 +7543,7 @@
         </is>
       </c>
       <c r="E296" t="n">
-        <v>0.09706392935315873</v>
+        <v>9.706392935315874</v>
       </c>
       <c r="F296" t="n">
         <v>0</v>
@@ -7567,7 +7567,7 @@
         </is>
       </c>
       <c r="E297" t="n">
-        <v>0.1333357573994619</v>
+        <v>13.33357573994619</v>
       </c>
       <c r="F297" t="n">
         <v>0</v>
@@ -7591,7 +7591,7 @@
         </is>
       </c>
       <c r="E298" t="n">
-        <v>0.09541019154318757</v>
+        <v>9.541019154318757</v>
       </c>
       <c r="F298" t="n">
         <v>0</v>
@@ -7615,7 +7615,7 @@
         </is>
       </c>
       <c r="E299" t="n">
-        <v>0.09538471949651485</v>
+        <v>9.538471949651486</v>
       </c>
       <c r="F299" t="n">
         <v>0</v>
@@ -7639,7 +7639,7 @@
         </is>
       </c>
       <c r="E300" t="n">
-        <v>0.0938529088913282</v>
+        <v>9.38529088913282</v>
       </c>
       <c r="F300" t="n">
         <v>1</v>
@@ -7663,7 +7663,7 @@
         </is>
       </c>
       <c r="E301" t="n">
-        <v>0.09249235114144505</v>
+        <v>9.249235114144504</v>
       </c>
       <c r="F301" t="n">
         <v>0</v>
@@ -7687,7 +7687,7 @@
         </is>
       </c>
       <c r="E302" t="n">
-        <v>0.09698081627397966</v>
+        <v>9.698081627397965</v>
       </c>
       <c r="F302" t="n">
         <v>0</v>
@@ -7711,7 +7711,7 @@
         </is>
       </c>
       <c r="E303" t="n">
-        <v>0.09346259963212752</v>
+        <v>9.346259963212752</v>
       </c>
       <c r="F303" t="n">
         <v>0</v>
@@ -7735,7 +7735,7 @@
         </is>
       </c>
       <c r="E304" t="n">
-        <v>0.09300701870429574</v>
+        <v>9.300701870429574</v>
       </c>
       <c r="F304" t="n">
         <v>1</v>
@@ -7759,7 +7759,7 @@
         </is>
       </c>
       <c r="E305" t="n">
-        <v>0.09239580458183826</v>
+        <v>9.239580458183825</v>
       </c>
       <c r="F305" t="n">
         <v>0</v>
@@ -7783,7 +7783,7 @@
         </is>
       </c>
       <c r="E306" t="n">
-        <v>0.09374886227108895</v>
+        <v>9.374886227108895</v>
       </c>
       <c r="F306" t="n">
         <v>0</v>
@@ -7807,7 +7807,7 @@
         </is>
       </c>
       <c r="E307" t="n">
-        <v>0.09379448313007348</v>
+        <v>9.379448313007348</v>
       </c>
       <c r="F307" t="n">
         <v>0</v>
@@ -7831,7 +7831,7 @@
         </is>
       </c>
       <c r="E308" t="n">
-        <v>0.09553933495539335</v>
+        <v>9.553933495539335</v>
       </c>
       <c r="F308" t="n">
         <v>0</v>
@@ -7855,7 +7855,7 @@
         </is>
       </c>
       <c r="E309" t="n">
-        <v>0.1002591189954156</v>
+        <v>10.02591189954156</v>
       </c>
       <c r="F309" t="n">
         <v>1</v>
@@ -7879,7 +7879,7 @@
         </is>
       </c>
       <c r="E310" t="n">
-        <v>0.09296804341272234</v>
+        <v>9.296804341272233</v>
       </c>
       <c r="F310" t="n">
         <v>0</v>
@@ -7903,7 +7903,7 @@
         </is>
       </c>
       <c r="E311" t="n">
-        <v>0.09645131938125569</v>
+        <v>9.645131938125569</v>
       </c>
       <c r="F311" t="n">
         <v>0</v>
@@ -7927,7 +7927,7 @@
         </is>
       </c>
       <c r="E312" t="n">
-        <v>0.09935095401939319</v>
+        <v>9.935095401939318</v>
       </c>
       <c r="F312" t="n">
         <v>0</v>
@@ -7951,7 +7951,7 @@
         </is>
       </c>
       <c r="E313" t="n">
-        <v>0.09211724012379392</v>
+        <v>9.211724012379392</v>
       </c>
       <c r="F313" t="n">
         <v>1</v>
@@ -7975,7 +7975,7 @@
         </is>
       </c>
       <c r="E314" t="n">
-        <v>0.09925362914270063</v>
+        <v>9.925362914270062</v>
       </c>
       <c r="F314" t="n">
         <v>0</v>
@@ -7999,7 +7999,7 @@
         </is>
       </c>
       <c r="E315" t="n">
-        <v>0.09697361509555942</v>
+        <v>9.697361509555941</v>
       </c>
       <c r="F315" t="n">
         <v>0</v>
@@ -8023,7 +8023,7 @@
         </is>
       </c>
       <c r="E316" t="n">
-        <v>0.09587451482533713</v>
+        <v>9.587451482533712</v>
       </c>
       <c r="F316" t="n">
         <v>0</v>
@@ -8047,7 +8047,7 @@
         </is>
       </c>
       <c r="E317" t="n">
-        <v>0.09807312252964427</v>
+        <v>9.807312252964428</v>
       </c>
       <c r="F317" t="n">
         <v>0</v>
@@ -8071,7 +8071,7 @@
         </is>
       </c>
       <c r="E318" t="n">
-        <v>0.09235703611910923</v>
+        <v>9.235703611910923</v>
       </c>
       <c r="F318" t="n">
         <v>0</v>
@@ -8095,7 +8095,7 @@
         </is>
       </c>
       <c r="E319" t="n">
-        <v>0.09192513970670967</v>
+        <v>9.192513970670966</v>
       </c>
       <c r="F319" t="n">
         <v>0</v>
@@ -8119,7 +8119,7 @@
         </is>
       </c>
       <c r="E320" t="n">
-        <v>0.09835769716657643</v>
+        <v>9.835769716657643</v>
       </c>
       <c r="F320" t="n">
         <v>0</v>
@@ -8143,7 +8143,7 @@
         </is>
       </c>
       <c r="E321" t="n">
-        <v>0.09625160143819482</v>
+        <v>9.625160143819482</v>
       </c>
       <c r="F321" t="n">
         <v>0</v>
@@ -8167,7 +8167,7 @@
         </is>
       </c>
       <c r="E322" t="n">
-        <v>0.09346980877568833</v>
+        <v>9.346980877568834</v>
       </c>
       <c r="F322" t="n">
         <v>1</v>
@@ -8191,7 +8191,7 @@
         </is>
       </c>
       <c r="E323" t="n">
-        <v>0.09535142604890408</v>
+        <v>9.535142604890408</v>
       </c>
       <c r="F323" t="n">
         <v>0</v>
@@ -8215,7 +8215,7 @@
         </is>
       </c>
       <c r="E324" t="n">
-        <v>0.0975609756097561</v>
+        <v>9.75609756097561</v>
       </c>
       <c r="F324" t="n">
         <v>1</v>
@@ -8239,7 +8239,7 @@
         </is>
       </c>
       <c r="E325" t="n">
-        <v>0.9361619307123394</v>
+        <v>93.61619307123394</v>
       </c>
       <c r="F325" t="n">
         <v>0</v>
@@ -8263,7 +8263,7 @@
         </is>
       </c>
       <c r="E326" t="n">
-        <v>0.0972246773908432</v>
+        <v>9.722467739084321</v>
       </c>
       <c r="F326" t="n">
         <v>1</v>
@@ -8287,7 +8287,7 @@
         </is>
       </c>
       <c r="E327" t="n">
-        <v>0.09506613649273715</v>
+        <v>9.506613649273715</v>
       </c>
       <c r="F327" t="n">
         <v>0</v>
@@ -8311,7 +8311,7 @@
         </is>
       </c>
       <c r="E328" t="n">
-        <v>0.09466761613538306</v>
+        <v>9.466761613538306</v>
       </c>
       <c r="F328" t="n">
         <v>1</v>
@@ -8335,7 +8335,7 @@
         </is>
       </c>
       <c r="E329" t="n">
-        <v>0.09375610900418345</v>
+        <v>9.375610900418344</v>
       </c>
       <c r="F329" t="n">
         <v>0</v>
@@ -8359,7 +8359,7 @@
         </is>
       </c>
       <c r="E330" t="n">
-        <v>0.09502008379043753</v>
+        <v>9.502008379043753</v>
       </c>
       <c r="F330" t="n">
         <v>0</v>
@@ -8383,7 +8383,7 @@
         </is>
       </c>
       <c r="E331" t="n">
-        <v>0.09617593262154919</v>
+        <v>9.617593262154919</v>
       </c>
       <c r="F331" t="n">
         <v>0</v>
@@ -8407,7 +8407,7 @@
         </is>
       </c>
       <c r="E332" t="n">
-        <v>0.09590746616329973</v>
+        <v>9.590746616329973</v>
       </c>
       <c r="F332" t="n">
         <v>0</v>
@@ -8431,7 +8431,7 @@
         </is>
       </c>
       <c r="E333" t="n">
-        <v>0.08788150384452097</v>
+        <v>8.788150384452097</v>
       </c>
       <c r="F333" t="n">
         <v>0</v>
@@ -8455,7 +8455,7 @@
         </is>
       </c>
       <c r="E334" t="n">
-        <v>0.09158206429780034</v>
+        <v>9.158206429780034</v>
       </c>
       <c r="F334" t="n">
         <v>0</v>
@@ -8479,7 +8479,7 @@
         </is>
       </c>
       <c r="E335" t="n">
-        <v>0.09646925367490665</v>
+        <v>9.646925367490665</v>
       </c>
       <c r="F335" t="n">
         <v>1</v>
@@ -8503,7 +8503,7 @@
         </is>
       </c>
       <c r="E336" t="n">
-        <v>0.09399728938049229</v>
+        <v>9.399728938049229</v>
       </c>
       <c r="F336" t="n">
         <v>1</v>
@@ -8527,7 +8527,7 @@
         </is>
       </c>
       <c r="E337" t="n">
-        <v>0.09227832870005394</v>
+        <v>9.227832870005393</v>
       </c>
       <c r="F337" t="n">
         <v>0</v>
@@ -8551,7 +8551,7 @@
         </is>
       </c>
       <c r="E338" t="n">
-        <v>0.09834805993084902</v>
+        <v>9.834805993084903</v>
       </c>
       <c r="F338" t="n">
         <v>1</v>
@@ -8575,7 +8575,7 @@
         </is>
       </c>
       <c r="E339" t="n">
-        <v>0.09591450216450216</v>
+        <v>9.591450216450216</v>
       </c>
       <c r="F339" t="n">
         <v>0</v>
@@ -8599,7 +8599,7 @@
         </is>
       </c>
       <c r="E340" t="n">
-        <v>0.09348137535816618</v>
+        <v>9.348137535816619</v>
       </c>
       <c r="F340" t="n">
         <v>0</v>
@@ -8623,7 +8623,7 @@
         </is>
       </c>
       <c r="E341" t="n">
-        <v>0.09510060452945954</v>
+        <v>9.510060452945954</v>
       </c>
       <c r="F341" t="n">
         <v>0</v>
@@ -8647,7 +8647,7 @@
         </is>
       </c>
       <c r="E342" t="n">
-        <v>0.09311803152633602</v>
+        <v>9.311803152633601</v>
       </c>
       <c r="F342" t="n">
         <v>0</v>
@@ -8671,7 +8671,7 @@
         </is>
       </c>
       <c r="E343" t="n">
-        <v>0.09367361312507769</v>
+        <v>9.367361312507768</v>
       </c>
       <c r="F343" t="n">
         <v>0</v>
@@ -8695,7 +8695,7 @@
         </is>
       </c>
       <c r="E344" t="n">
-        <v>0.09179440937781785</v>
+        <v>9.179440937781786</v>
       </c>
       <c r="F344" t="n">
         <v>0</v>
@@ -8719,7 +8719,7 @@
         </is>
       </c>
       <c r="E345" t="n">
-        <v>0.0992679355783309</v>
+        <v>9.92679355783309</v>
       </c>
       <c r="F345" t="n">
         <v>1</v>
@@ -8743,7 +8743,7 @@
         </is>
       </c>
       <c r="E346" t="n">
-        <v>0.09627569859142089</v>
+        <v>9.627569859142088</v>
       </c>
       <c r="F346" t="n">
         <v>1</v>
@@ -8767,7 +8767,7 @@
         </is>
       </c>
       <c r="E347" t="n">
-        <v>0.09422612297224003</v>
+        <v>9.422612297224003</v>
       </c>
       <c r="F347" t="n">
         <v>0</v>
@@ -8791,7 +8791,7 @@
         </is>
       </c>
       <c r="E348" t="n">
-        <v>0.1004243281471004</v>
+        <v>10.04243281471004</v>
       </c>
       <c r="F348" t="n">
         <v>0</v>
@@ -8815,7 +8815,7 @@
         </is>
       </c>
       <c r="E349" t="n">
-        <v>0.1020938483833891</v>
+        <v>10.20938483833891</v>
       </c>
       <c r="F349" t="n">
         <v>0</v>
@@ -8839,7 +8839,7 @@
         </is>
       </c>
       <c r="E350" t="n">
-        <v>0.09636476842760669</v>
+        <v>9.636476842760668</v>
       </c>
       <c r="F350" t="n">
         <v>1</v>
@@ -8863,7 +8863,7 @@
         </is>
       </c>
       <c r="E351" t="n">
-        <v>0.09608134920634921</v>
+        <v>9.608134920634921</v>
       </c>
       <c r="F351" t="n">
         <v>0</v>
@@ -8887,7 +8887,7 @@
         </is>
       </c>
       <c r="E352" t="n">
-        <v>0.09594520273986301</v>
+        <v>9.594520273986301</v>
       </c>
       <c r="F352" t="n">
         <v>0</v>
@@ -8911,7 +8911,7 @@
         </is>
       </c>
       <c r="E353" t="n">
-        <v>0.09304848141860027</v>
+        <v>9.304848141860028</v>
       </c>
       <c r="F353" t="n">
         <v>0</v>
@@ -8935,7 +8935,7 @@
         </is>
       </c>
       <c r="E354" t="n">
-        <v>0.09317958783120707</v>
+        <v>9.317958783120707</v>
       </c>
       <c r="F354" t="n">
         <v>0</v>

</xml_diff>